<commit_message>
Adjusting StudentDTORowMapper, and removing used files
</commit_message>
<xml_diff>
--- a/src/main/resources/data/students.xlsx
+++ b/src/main/resources/data/students.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcosta\Documents\Repository-local\excel-reader\src\main\resources\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcosta\Documents\Repository-local\excel-reader\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,30 +29,6 @@
     <t xml:space="preserve">NAME            </t>
   </si>
   <si>
-    <t xml:space="preserve">Tony </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nick </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ian </t>
-  </si>
-  <si>
-    <t>EMAIL_ADDRESS</t>
-  </si>
-  <si>
-    <t>PURCHASED_PACKAGE</t>
-  </si>
-  <si>
-    <t>tony.tester@gmail.com</t>
-  </si>
-  <si>
-    <t>nick.newbie@gmail.com</t>
-  </si>
-  <si>
-    <t>ian.intermediate@gmail.com</t>
-  </si>
-  <si>
     <t>master</t>
   </si>
   <si>
@@ -60,13 +36,37 @@
   </si>
   <si>
     <t>intermediate</t>
+  </si>
+  <si>
+    <t>marcioc424@gmail.com</t>
+  </si>
+  <si>
+    <t>teste@gmail.com</t>
+  </si>
+  <si>
+    <t>teste2@gmail.com</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>Marcio</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Teste 2</t>
+  </si>
+  <si>
+    <t>LEVEL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,12 +76,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -107,12 +101,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,7 +389,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,48 +402,53 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>